<commit_message>
feat: add new event
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/Standalone.xlsx
+++ b/examples/test/testFiles/Standalone.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E1FE25-0883-4634-B89E-839B5F57775E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C00646-26CF-A74A-9DED-E85D78AB21C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="2175" windowWidth="21600" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="1460" windowWidth="21600" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>product_ID</t>
   </si>
@@ -413,12 +414,12 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,7 +427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>253</v>
       </c>
@@ -438,7 +439,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>254</v>
       </c>
@@ -454,4 +455,43 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E851F89-7DA8-D646-86B3-E7D98E35611C}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>253</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>254</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add sheet name to payload  (#346)
* feat: support multiple sheets in upload

stores sheet name in column data

* fix: always concat

* feat: add new event

---------

Co-authored-by: Ogulcan <ogul247@gmail.com>
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/Standalone.xlsx
+++ b/examples/test/testFiles/Standalone.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E1FE25-0883-4634-B89E-839B5F57775E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C00646-26CF-A74A-9DED-E85D78AB21C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="2175" windowWidth="21600" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="1460" windowWidth="21600" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>product_ID</t>
   </si>
@@ -413,12 +414,12 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,7 +427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>253</v>
       </c>
@@ -438,7 +439,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>254</v>
       </c>
@@ -454,4 +455,43 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E851F89-7DA8-D646-86B3-E7D98E35611C}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>253</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>254</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>